<commit_message>
get data from senate
</commit_message>
<xml_diff>
--- a/data/Fim do Foro.xlsx
+++ b/data/Fim do Foro.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Camara" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Senado" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7182" uniqueCount="3141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8248" uniqueCount="3624">
   <si>
     <t>e-mail *</t>
   </si>
@@ -9434,6 +9435,1455 @@
   </si>
   <si>
     <t>http://www.camara.gov.br/internet/deputado/bandep/178949.jpg</t>
+  </si>
+  <si>
+    <t>gladson.cameli@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Gladson de Lima Cameli</t>
+  </si>
+  <si>
+    <t>Gladson Cameli</t>
+  </si>
+  <si>
+    <t>(61) 3303-1357 / 1367</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 14</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4558.jpg</t>
+  </si>
+  <si>
+    <t>jorge.viana@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Contra</t>
+  </si>
+  <si>
+    <t>Jorge Ney Viana Macedo Neves</t>
+  </si>
+  <si>
+    <t>Jorge Viana</t>
+  </si>
+  <si>
+    <t>(61) 3303-6366 / 6369</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco B Ala Ruy Carneiro Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4990.jpg</t>
+  </si>
+  <si>
+    <t>sergio.petecao@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Sérgio de Oliveira Cunha</t>
+  </si>
+  <si>
+    <t>Sérgio Petecão</t>
+  </si>
+  <si>
+    <t>(61) 3303-6708 / 6709</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 21</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4560.jpg</t>
+  </si>
+  <si>
+    <t>benedito.lira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Benedito de Lira</t>
+  </si>
+  <si>
+    <t>(61) 3303-6148 / 6149 / 6151</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 02</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3823.jpg</t>
+  </si>
+  <si>
+    <t>fernando.collor@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Fernando Affonso Collor de Mello</t>
+  </si>
+  <si>
+    <t>Fernando Collor</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>(61) 3303-5783</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 13º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4525.jpg</t>
+  </si>
+  <si>
+    <t>renan.calheiros@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Renan Vasconcelos Calheiros</t>
+  </si>
+  <si>
+    <t>Renan Calheiros</t>
+  </si>
+  <si>
+    <t>(61) 3303-2261</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 15º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador70.jpg</t>
+  </si>
+  <si>
+    <t>davi.alcolumbre@senador.leg.br</t>
+  </si>
+  <si>
+    <t>David Samuel Alcolumbre Tobelem</t>
+  </si>
+  <si>
+    <t>Davi Alcolumbre</t>
+  </si>
+  <si>
+    <t>(61) 3303-6717 / 6720 / 6722</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 03</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3830.jpg</t>
+  </si>
+  <si>
+    <t>joao.capiberibe@senador.leg.br</t>
+  </si>
+  <si>
+    <t>João Alberto Rodrigues Capiberibe</t>
+  </si>
+  <si>
+    <t>João Capiberibe</t>
+  </si>
+  <si>
+    <t>(61) 3303-9011 / 9013</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 08</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3394.jpg</t>
+  </si>
+  <si>
+    <t>randolfe.rodrigues@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Randolph Frederich Rodrigues Alves</t>
+  </si>
+  <si>
+    <t>Randolfe Rodrigues</t>
+  </si>
+  <si>
+    <t>(61) 3303-6568 / 6567 / 6574</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 07</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5012.jpg</t>
+  </si>
+  <si>
+    <t>eduardo.braga@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo de Souza Braga</t>
+  </si>
+  <si>
+    <t>Eduardo Braga</t>
+  </si>
+  <si>
+    <t>(61) 3303-6230 / 6227</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 12º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4994.jpg</t>
+  </si>
+  <si>
+    <t>omar.aziz@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Omar José Abdel Aziz</t>
+  </si>
+  <si>
+    <t>Omar Aziz</t>
+  </si>
+  <si>
+    <t>(61) 3303-6579</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Filinto Müller Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5525.jpg</t>
+  </si>
+  <si>
+    <t>vanessa.grazziotin@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Vanessa Grazziotin</t>
+  </si>
+  <si>
+    <t>(61) 3303-6726 / 6733</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Alexandre Costa Gabinete 03</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador558.jpg</t>
+  </si>
+  <si>
+    <t>lidice.mata@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Lídice da Mata e Souza</t>
+  </si>
+  <si>
+    <t>Lídice da Mata</t>
+  </si>
+  <si>
+    <t>(61) 3303-6408 / 6410</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 15</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4575.jpg</t>
+  </si>
+  <si>
+    <t>otto.alencar@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Otto Roberto Mendonça de Alencar</t>
+  </si>
+  <si>
+    <t>Otto Alencar</t>
+  </si>
+  <si>
+    <t>(61) 3303-1464 / 1467</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 09</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5523.jpg</t>
+  </si>
+  <si>
+    <t>roberto.muniz@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Roberto de Oliveira Muniz</t>
+  </si>
+  <si>
+    <t>Roberto Muniz</t>
+  </si>
+  <si>
+    <t>(61) 3303-6788 / 6790</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 13</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5052.jpg</t>
+  </si>
+  <si>
+    <t>eunicio.oliveira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Eunício Lopes de Oliveira</t>
+  </si>
+  <si>
+    <t>Eunício Oliveira</t>
+  </si>
+  <si>
+    <t>(61) 3303-6245 / 6246</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 17º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador612.jpg</t>
+  </si>
+  <si>
+    <t>jose.pimentel@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Barroso Pimentel</t>
+  </si>
+  <si>
+    <t>José Pimentel</t>
+  </si>
+  <si>
+    <t>(61) 3303-6390 / 6391</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 23º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador615.jpg</t>
+  </si>
+  <si>
+    <t>tasso.jereissati@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Tasso Ribeiro Jereissati</t>
+  </si>
+  <si>
+    <t>Tasso Jereissati</t>
+  </si>
+  <si>
+    <t>(61) 3303-4502 / 4503</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 14º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3396.jpg</t>
+  </si>
+  <si>
+    <t>cristovam.buarque@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Cristovam Ricardo Cavalcanti Buarque</t>
+  </si>
+  <si>
+    <t>Cristovam Buarque</t>
+  </si>
+  <si>
+    <t>(61) 3303-2281</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 10</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3398.jpg</t>
+  </si>
+  <si>
+    <t>heliojose@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Hélio José da Silva Lima</t>
+  </si>
+  <si>
+    <t>Hélio José</t>
+  </si>
+  <si>
+    <t>(61) 3303-6640 / 6645 / 6646</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 19</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5100.jpg</t>
+  </si>
+  <si>
+    <t>reguffe@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Antônio Machado Reguffe</t>
+  </si>
+  <si>
+    <t>Reguffe</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>(61) 3303-6355</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 17</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5236.jpg</t>
+  </si>
+  <si>
+    <t>magno.malta@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Magno Pereira Malta</t>
+  </si>
+  <si>
+    <t>Magno Malta</t>
+  </si>
+  <si>
+    <t>(61) 3303-4161 / 5867</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Tancredo Neves Gabinete 57</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador631.jpg</t>
+  </si>
+  <si>
+    <t>ricardo.ferraco@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ricardo de Rezende Ferraço</t>
+  </si>
+  <si>
+    <t>Ricardo Ferraço</t>
+  </si>
+  <si>
+    <t>(61) 3303-6590 / 6593</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 4º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador635.jpg</t>
+  </si>
+  <si>
+    <t>rose.freitas@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Rosilda de Freitas</t>
+  </si>
+  <si>
+    <t>Rose de Freitas</t>
+  </si>
+  <si>
+    <t>(61) 3303-1156</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador2331.jpg</t>
+  </si>
+  <si>
+    <t>lucia.vania@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Lúcia Vânia Abrão</t>
+  </si>
+  <si>
+    <t>Lúcia Vânia</t>
+  </si>
+  <si>
+    <t>(61) 3303-2844 / 2035</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 16</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador643.jpg</t>
+  </si>
+  <si>
+    <t>ronaldo.caiado@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ronaldo Ramos Caiado</t>
+  </si>
+  <si>
+    <t>Ronaldo Caiado</t>
+  </si>
+  <si>
+    <t>(61) 3303-6439 / 6440 / 6445</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Alexandre Costa Gabinete 21</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador456.jpg</t>
+  </si>
+  <si>
+    <t>wilder.morais@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Wilder Pedro de Morais</t>
+  </si>
+  <si>
+    <t>Wilder Morais</t>
+  </si>
+  <si>
+    <t>(61) 3303-2092 / 2093 / 1809 / 2099 / 2964</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Afonso Arinos Gabinete 13</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5070.jpg</t>
+  </si>
+  <si>
+    <t>edison.lobao@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Edison Lobão</t>
+  </si>
+  <si>
+    <t>(61) 3303-2311 / 2312 / 1989</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Tancredo Neves Gabinete 54</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador16.jpg</t>
+  </si>
+  <si>
+    <t>joao.alberto.souza@senador.leg.br</t>
+  </si>
+  <si>
+    <t>João Alberto de Souza</t>
+  </si>
+  <si>
+    <t>João Alberto Souza</t>
+  </si>
+  <si>
+    <t>(61) 3303-6349 / 6352</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 5º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador950.jpg</t>
+  </si>
+  <si>
+    <t>robertorocha@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Roberto Coelho Rocha</t>
+  </si>
+  <si>
+    <t>Roberto Rocha</t>
+  </si>
+  <si>
+    <t>(61) 3303-1437 / 1506</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 25º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador677.jpg</t>
+  </si>
+  <si>
+    <t>cidinho.santos@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Aparecido dos Santos</t>
+  </si>
+  <si>
+    <t>Cidinho Santos</t>
+  </si>
+  <si>
+    <t>(61) 3303-6167 / 6161 / 6172 / 6168</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 19º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5108.jpg</t>
+  </si>
+  <si>
+    <t>josemedeiros@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Antônio Medeiros</t>
+  </si>
+  <si>
+    <t>José Medeiros</t>
+  </si>
+  <si>
+    <t>(61) 3303-1146 / 1148</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 04</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5112.jpg</t>
+  </si>
+  <si>
+    <t>wellington.fagundes@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Wellington Antonio Fagundes</t>
+  </si>
+  <si>
+    <t>Wellington Fagundes</t>
+  </si>
+  <si>
+    <t>(61) 3303-6219 / 6213 / 6221</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco B Ala Ruy Carneiro Gabinete 04</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador1173.jpg</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pedro Chaves dos Santos Filho</t>
+  </si>
+  <si>
+    <t>Pedro Chaves</t>
+  </si>
+  <si>
+    <t>(61) 3303-2453 / 2454 / 2455 / 2456 / 2457</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 02</t>
+  </si>
+  <si>
+    <t>http://senadorpedrochaves.com.br/</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5116.jpg</t>
+  </si>
+  <si>
+    <t>simone.tebet@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Simone Nassar Tebet</t>
+  </si>
+  <si>
+    <t>Simone Tebet</t>
+  </si>
+  <si>
+    <t>(61) 3303-1128</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 11</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5527.jpg</t>
+  </si>
+  <si>
+    <t>waldemir.moka@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Waldemir Moka Miranda de Britto</t>
+  </si>
+  <si>
+    <t>Waldemir Moka</t>
+  </si>
+  <si>
+    <t>(61) 3303-6767 / 6768 / 6774</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 24º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador1176.jpg</t>
+  </si>
+  <si>
+    <t>aecio.neves@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Aécio Neves da Cunha</t>
+  </si>
+  <si>
+    <t>Aécio Neves</t>
+  </si>
+  <si>
+    <t>(61) 3303-6049 / 6050</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 11º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador391.jpg</t>
+  </si>
+  <si>
+    <t>antonio.anastasia@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Antonio Augusto Junho Anastasia</t>
+  </si>
+  <si>
+    <t>Antonio Anastasia</t>
+  </si>
+  <si>
+    <t>(61) 3303-5717</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 23</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5529.jpg</t>
+  </si>
+  <si>
+    <t>zeze.perrella@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Perrella de Oliveira Costa</t>
+  </si>
+  <si>
+    <t>Zeze Perrella</t>
+  </si>
+  <si>
+    <t>(61) 3303-2191 / 2192</t>
+  </si>
+  <si>
+    <t>Senado Federal Edifício Principal Ala Antônio Carlos Magalhãe Gabinete 05</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5144.jpg</t>
+  </si>
+  <si>
+    <t>flexa.ribeiro@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Fernando de Souza Flexa Ribeiro</t>
+  </si>
+  <si>
+    <t>Flexa Ribeiro</t>
+  </si>
+  <si>
+    <t>(61) 3303-2342</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Tancredo Neves Gabinete 51</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3634.jpg</t>
+  </si>
+  <si>
+    <t>jader.barbalho@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Jader Fontenelle Barbalho</t>
+  </si>
+  <si>
+    <t>Jader Barbalho</t>
+  </si>
+  <si>
+    <t>(61) 3303-9826 / 9831 / 9827 / 9832</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 2º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador35.jpg</t>
+  </si>
+  <si>
+    <t>paulo.rocha@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Paulo Roberto Galvão da Rocha</t>
+  </si>
+  <si>
+    <t>Paulo Rocha</t>
+  </si>
+  <si>
+    <t>(61) 3303-3800</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 08</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador374.jpg</t>
+  </si>
+  <si>
+    <t>cassio.cunha.lima@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Cássio Rodrigues da Cunha Lima</t>
+  </si>
+  <si>
+    <t>Cássio Cunha Lima</t>
+  </si>
+  <si>
+    <t>(61) 3303-9808 / 9809 / 9810</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 10º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5197.jpg</t>
+  </si>
+  <si>
+    <t>jose.maranhao@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Targino Maranhão</t>
+  </si>
+  <si>
+    <t>José Maranhão</t>
+  </si>
+  <si>
+    <t>(61) 3303-6490 / 6485</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 7º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3361.jpg</t>
+  </si>
+  <si>
+    <t>raimundo.lira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Raimundo Lira</t>
+  </si>
+  <si>
+    <t>(61) 3303-6747 / 6754</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 18º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador2207.jpg</t>
+  </si>
+  <si>
+    <t>alvarodias@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Alvaro Fernandes Dias</t>
+  </si>
+  <si>
+    <t>Alvaro Dias</t>
+  </si>
+  <si>
+    <t>(61) 3303-4059 / 4060</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Nilo Coelho Gabinete 10</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador945.jpg</t>
+  </si>
+  <si>
+    <t>gleisi@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Gleisi Helena Hoffmann</t>
+  </si>
+  <si>
+    <t>Gleisi Hoffmann</t>
+  </si>
+  <si>
+    <t>(61) 3303-6265</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 04</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5006.jpg</t>
+  </si>
+  <si>
+    <t>roberto.requiao@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Roberto Requião de Mello e Silva</t>
+  </si>
+  <si>
+    <t>Roberto Requião</t>
+  </si>
+  <si>
+    <t>(61) 3303-6623 / 6624 / 6621 / 6625</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 18</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador72.jpg</t>
+  </si>
+  <si>
+    <t>armando.monteiro@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Armando de Queiroz Monteiro Neto</t>
+  </si>
+  <si>
+    <t>Armando Monteiro</t>
+  </si>
+  <si>
+    <t>(61) 3303-6130 / 6127</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador715.jpg</t>
+  </si>
+  <si>
+    <t>fernandobezerracoelho@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Fernando Bezerra de Souza Coelho</t>
+  </si>
+  <si>
+    <t>Fernando Bezerra Coelho</t>
+  </si>
+  <si>
+    <t>(61) 3303-2182</t>
+  </si>
+  <si>
+    <t>Senado Federal Edifício Principal Ala Dinarte Mariz Gabinete 04</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5540.jpg</t>
+  </si>
+  <si>
+    <t>humberto.costa@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Humberto Sérgio Costa Lima</t>
+  </si>
+  <si>
+    <t>Humberto Costa</t>
+  </si>
+  <si>
+    <t>(61) 3303-6285 / 6286</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 25</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5008.jpg</t>
+  </si>
+  <si>
+    <t>ciro.nogueira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ciro Nogueira Lima Filho</t>
+  </si>
+  <si>
+    <t>Ciro Nogueira</t>
+  </si>
+  <si>
+    <t>(61) 3303-6187 / 6188</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 3º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador739.jpg</t>
+  </si>
+  <si>
+    <t>elmano.ferrer@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Elmano Férrer de Almeida</t>
+  </si>
+  <si>
+    <t>Elmano Férrer</t>
+  </si>
+  <si>
+    <t>(61) 3303-2415 / 3055 / 1015</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 06</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5531.jpg</t>
+  </si>
+  <si>
+    <t>reginasousa@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Maria Regina Sousa</t>
+  </si>
+  <si>
+    <t>Regina Sousa</t>
+  </si>
+  <si>
+    <t>(61) 3303-9049</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 06</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5182.jpg</t>
+  </si>
+  <si>
+    <t>eduardo.lopes@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Eduardo Benedito Lopes</t>
+  </si>
+  <si>
+    <t>Eduardo Lopes</t>
+  </si>
+  <si>
+    <t>(61) 3303-5730 / 5225</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Ruy Carneiro Gabinete 02</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4767.jpg</t>
+  </si>
+  <si>
+    <t>lindbergh.farias@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Luiz Lindbergh Farias Filho</t>
+  </si>
+  <si>
+    <t>Lindbergh Farias</t>
+  </si>
+  <si>
+    <t>(61) 3303-6426 / 6427</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 11</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3695.jpg</t>
+  </si>
+  <si>
+    <t>romario@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Romario de Souza Faria</t>
+  </si>
+  <si>
+    <t>Romário</t>
+  </si>
+  <si>
+    <t>(61) 3303-6519 / 6517</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Nilo Coelho Gabinete 11</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5322.jpg</t>
+  </si>
+  <si>
+    <t>fatima.bezerra@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Maria de Fátima Bezerra</t>
+  </si>
+  <si>
+    <t>Fátima Bezerra</t>
+  </si>
+  <si>
+    <t>(61) 3303-1777 / 1884</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 03</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3713.jpg</t>
+  </si>
+  <si>
+    <t>garibaldi.alves@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Garibaldi Alves Filho</t>
+  </si>
+  <si>
+    <t>(61) 3303-2371 / 2372</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 8º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador87.jpg</t>
+  </si>
+  <si>
+    <t>jose.agripino@senador.leg.br</t>
+  </si>
+  <si>
+    <t>José Agripino Maia</t>
+  </si>
+  <si>
+    <t>José Agripino</t>
+  </si>
+  <si>
+    <t>(61) 3303-2366 / 2361 / 2362</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 09</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador40.jpg</t>
+  </si>
+  <si>
+    <t>ana.amelia@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Ana Amélia de Lemos</t>
+  </si>
+  <si>
+    <t>Ana Amélia</t>
+  </si>
+  <si>
+    <t>(61) 3303-6083</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 07</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4988.jpg</t>
+  </si>
+  <si>
+    <t>lasier.martins@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Lasier Costa Martins</t>
+  </si>
+  <si>
+    <t>Lasier Martins</t>
+  </si>
+  <si>
+    <t>(61) 3303-2323</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Tancredo Neves Gabinete 50</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5533.jpg</t>
+  </si>
+  <si>
+    <t>paulopaim@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Paulo Renato Paim</t>
+  </si>
+  <si>
+    <t>Paulo Paim</t>
+  </si>
+  <si>
+    <t>(61) 3303-5232 / 5231 / 5230</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 22º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador825.jpg</t>
+  </si>
+  <si>
+    <t>acir@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Acir Marcos Gurgacz</t>
+  </si>
+  <si>
+    <t>Acir Gurgacz</t>
+  </si>
+  <si>
+    <t>(61) 3303-3132 / 3131</t>
+  </si>
+  <si>
+    <t>Senado Federal Edifício Principal Ala Dinarte Mariz Gabinete 05</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4981.jpg</t>
+  </si>
+  <si>
+    <t>ivo.cassol@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ivo Narciso Cassol</t>
+  </si>
+  <si>
+    <t>Ivo Cassol</t>
+  </si>
+  <si>
+    <t>(61) 3303-6328 / 6329</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 16º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5004.jpg</t>
+  </si>
+  <si>
+    <t>valdir.raupp@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Valdir Raupp de Matos</t>
+  </si>
+  <si>
+    <t>Valdir Raupp</t>
+  </si>
+  <si>
+    <t>(61) 3303-2252 / 2253</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 20º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3372.jpg</t>
+  </si>
+  <si>
+    <t>angela.portela@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Angela Maria Gomes Portela</t>
+  </si>
+  <si>
+    <t>Angela Portela</t>
+  </si>
+  <si>
+    <t>(61) 3303-6103 / 6104 / 6105</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 10</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4697.jpg</t>
+  </si>
+  <si>
+    <t>romero.juca@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Romero Jucá Filho</t>
+  </si>
+  <si>
+    <t>Romero Jucá</t>
+  </si>
+  <si>
+    <t>(61) 3303-2115 / 2111 / 2119</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Afonso Arinos Gabinete 12</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador73.jpg</t>
+  </si>
+  <si>
+    <t>telmariomota@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Telmário Mota de Oliveira</t>
+  </si>
+  <si>
+    <t>Telmário Mota</t>
+  </si>
+  <si>
+    <t>(61) 3303-6315</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco B Ala Ruy Carneiro Gabinete 03</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5535.jpg</t>
+  </si>
+  <si>
+    <t>dalirio.beber@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Dalírio José Beber</t>
+  </si>
+  <si>
+    <t>Dalirio Beber</t>
+  </si>
+  <si>
+    <t>(61) 3303-6446 / 6447</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Nilo Coelho Sala 2</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5132.jpg</t>
+  </si>
+  <si>
+    <t>dario.berger@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Dário Elias Berger</t>
+  </si>
+  <si>
+    <t>Dário Berger</t>
+  </si>
+  <si>
+    <t>(61) 3303-5947 / 5951</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Ala Teotônio Vilela Gabinete 26</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5537.jpg</t>
+  </si>
+  <si>
+    <t>paulo.bauer@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Paulo Roberto Bauer</t>
+  </si>
+  <si>
+    <t>Paulo Bauer</t>
+  </si>
+  <si>
+    <t>(61) 3303-6529 / 6530</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Afonso Arinos Gabinete 05</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3741.jpg</t>
+  </si>
+  <si>
+    <t>aloysionunes.ferreira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Aloysio Nunes Ferreira Filho</t>
+  </si>
+  <si>
+    <t>Aloysio Nunes Ferreira</t>
+  </si>
+  <si>
+    <t>(61) 3303-6063 / 6064</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 9º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador846.jpg</t>
+  </si>
+  <si>
+    <t>José Aníbal Peres de Pontes</t>
+  </si>
+  <si>
+    <t>José Aníbal</t>
+  </si>
+  <si>
+    <t>(61) 3303-6651 / 6655</t>
+  </si>
+  <si>
+    <t>Senado Federal Edifício Principal Ala Dinarte Mariz Gabinete 02</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador878.jpg</t>
+  </si>
+  <si>
+    <t>marta.suplicy@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Marta Teresa Suplicy</t>
+  </si>
+  <si>
+    <t>Marta Suplicy</t>
+  </si>
+  <si>
+    <t>(61) 3303-6510 / 6514</t>
+  </si>
+  <si>
+    <t>Senado Federal Edifício Principal Ala Dinarte Mariz Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5000.jpg</t>
+  </si>
+  <si>
+    <t>antoniocarlosvaladares@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Antonio Carlos Valadares</t>
+  </si>
+  <si>
+    <t>(61) 3303-2201 / 2203 / 2204 / 1786</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 12</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador3.jpg</t>
+  </si>
+  <si>
+    <t>eduardo.amorim@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Eduardo Alves do Amorim</t>
+  </si>
+  <si>
+    <t>Eduardo Amorim</t>
+  </si>
+  <si>
+    <t>(61) 3303-6205 / 6206 / 6207 / 6208 / 6209 / 6210 / 6211</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Térreo Ala Alexandre Costa Gabinete 01</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4721.jpg</t>
+  </si>
+  <si>
+    <t>ricardo.franco@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ricardo Barreto Franco</t>
+  </si>
+  <si>
+    <t>Ricardo Franco</t>
+  </si>
+  <si>
+    <t>(61) 3303-1306 / 4055</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Subsolo Ala Nilo Coelho Gabinete 08</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5635.jpg</t>
+  </si>
+  <si>
+    <t>ataides.oliveira@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Ataídes de Oliveira</t>
+  </si>
+  <si>
+    <t>Ataídes Oliveira</t>
+  </si>
+  <si>
+    <t>(61) 3303-2163 / 2164 / 2165</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo II Bloco A Ala Teotônio Vilela Gabinete 05</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador5164.jpg</t>
+  </si>
+  <si>
+    <t>katia.abreu@senadora.leg.br</t>
+  </si>
+  <si>
+    <t>Kátia Regina de Abreu</t>
+  </si>
+  <si>
+    <t>Kátia Abreu</t>
+  </si>
+  <si>
+    <t>(61) 3303-2464 / 2708 / 5771 / 2466</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 6º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador1249.jpg</t>
+  </si>
+  <si>
+    <t>vicentinho.alves@senador.leg.br</t>
+  </si>
+  <si>
+    <t>Vicente Alves de Oliveira</t>
+  </si>
+  <si>
+    <t>Vicentinho Alves</t>
+  </si>
+  <si>
+    <t>(61) 3303-6469 / 6467</t>
+  </si>
+  <si>
+    <t>Senado Federal Anexo I 21º Andar</t>
+  </si>
+  <si>
+    <t>http://www.senado.gov.br/senadores/img/fotos-oficiais/senador4763.jpg</t>
   </si>
 </sst>
 </file>
@@ -9522,6 +10972,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -9529,7 +10983,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.57"/>
+    <col customWidth="1" min="1" max="1" width="39.71"/>
     <col customWidth="1" min="3" max="3" width="27.43"/>
     <col customWidth="1" min="4" max="4" width="22.29"/>
   </cols>
@@ -32121,4 +33575,3387 @@
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="28.86"/>
+    <col customWidth="1" min="7" max="7" width="24.71"/>
+    <col customWidth="1" min="10" max="10" width="29.0"/>
+    <col customWidth="1" min="12" max="12" width="55.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>3141</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3142</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3143</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3144</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>3145</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>3146</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3149</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3150</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>3151</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>3152</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>3153</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3155</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3156</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>3157</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3158</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>3159</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3161</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3161</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3162</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>3163</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>3164</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>3165</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3166</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3167</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3168</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>3169</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>3170</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>3171</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>3172</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3173</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3174</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>3175</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>3176</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>3177</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>3178</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3179</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3180</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>3181</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>3182</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>3183</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3185</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>3186</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>3187</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>3188</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>3189</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3191</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3192</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>3193</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>3194</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>3195</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3197</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3198</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>3199</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>3200</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>3201</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3203</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3204</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>3205</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>3206</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>3207</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>3208</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3209</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3209</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>3210</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>3211</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>3212</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>3213</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>3214</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3215</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>3216</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>3217</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>3218</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>3220</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3221</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>3222</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>3223</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>3224</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>3225</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3226</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3227</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>3228</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>3229</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>3230</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>3231</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3232</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3233</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>3234</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>3235</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>3236</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>3237</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3238</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>3239</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>3240</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>3241</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>3242</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3244</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3245</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>3246</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>3247</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>3248</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>3249</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3250</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3251</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>3252</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>3253</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>3254</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>3255</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3256</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>3257</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>3258</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>3259</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>3260</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>3261</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3262</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3263</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>3264</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>3265</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>3266</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>3267</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>3268</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>3269</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3270</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>3271</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>3272</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>3273</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>3275</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3276</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>3278</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>3279</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>3280</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>3283</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>3284</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>3285</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>3287</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3288</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>3289</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>3290</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>3291</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3293</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3294</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>3295</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>3296</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>3297</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>3299</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3300</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>3301</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>3303</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>3305</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3305</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>3306</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>3307</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>3308</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>3309</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>3310</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>3311</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>3312</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>3313</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>3314</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>3316</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>3317</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>3318</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>3319</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>3320</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>3321</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>3323</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>3324</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>3325</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>3326</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3328</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>3329</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>3334</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>3335</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>3336</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>3337</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>3338</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3340</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>3341</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>3342</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>3343</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>3344</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>3345</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>3346</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>3348</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>3349</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>3350</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>3351</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>3353</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>3354</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>3355</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>3356</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>3357</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>3359</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>3360</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>3361</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>3362</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>3363</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>3364</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>3365</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>3366</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>3367</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>3368</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>3369</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>3371</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>3372</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>3373</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>3374</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>3375</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
+        <v>3376</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3377</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>3378</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>3379</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>3380</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>3381</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>3383</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>3384</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>3385</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>3386</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>3387</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>3388</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>3389</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>3390</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>3391</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>3392</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>3393</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>3394</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>3395</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>3396</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>3397</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>3398</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>3399</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>3400</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>3401</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>3402</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>3403</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>3404</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>3405</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>3406</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>3407</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>3407</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>3408</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>3409</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>3410</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>3411</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>3412</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>3413</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>3414</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>3415</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>3416</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>3417</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>3418</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>3419</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>3420</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>3421</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>3422</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="s">
+        <v>3423</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>3424</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>3425</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>3426</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>3427</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>3428</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>3429</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>3430</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>3431</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>3432</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>3433</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>3434</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>3435</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>3436</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>3437</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>3438</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>3439</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>3440</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>3441</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>3442</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>3443</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>3444</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>3445</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>3446</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>3447</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>3448</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>3449</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>3450</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>3451</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>3452</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
+        <v>3453</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>3454</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>3455</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>3456</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>3457</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>3458</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>3459</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>3460</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>3461</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>3462</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>3463</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>3464</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="s">
+        <v>3465</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>3466</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>3467</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>3468</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>3469</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>3470</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="s">
+        <v>3471</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>3472</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>3473</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>3474</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>3475</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>3476</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="s">
+        <v>3477</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>3478</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>3479</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>3480</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>3481</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>3482</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="s">
+        <v>3483</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>3484</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>3485</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>3486</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>3488</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="s">
+        <v>3489</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>3490</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>3490</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>3491</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>3492</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>3493</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="s">
+        <v>3494</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>3495</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>3497</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>3498</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>3499</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="s">
+        <v>3500</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>3501</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>3502</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>3503</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>3504</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>3505</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="s">
+        <v>3506</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>3507</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>3508</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>3509</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>3510</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>3511</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="s">
+        <v>3512</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>3513</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>3514</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>3515</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>3516</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>3517</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="s">
+        <v>3518</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>3519</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>3520</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>3521</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>3523</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="s">
+        <v>3524</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>3525</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>3526</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>3527</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>3528</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>3529</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="s">
+        <v>3530</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>3531</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>3532</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>3533</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>3534</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>3535</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="s">
+        <v>3536</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>3537</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>3538</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>3539</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>3540</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>3541</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="s">
+        <v>3542</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>3543</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>3544</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>3545</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>3546</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>3547</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="s">
+        <v>3548</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>3549</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>3550</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>3551</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>3552</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>3553</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="s">
+        <v>3554</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>3555</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>3556</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>3557</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>3558</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>3559</v>
+      </c>
+      <c r="M71" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="s">
+        <v>3560</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>3561</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>3562</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>3563</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>3564</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>3565</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="s">
+        <v>3566</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>3568</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>3569</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>3570</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>3571</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="s">
+        <v>3572</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>3573</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>3574</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>3575</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>3576</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>3577</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>3578</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>3579</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>3580</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>3581</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>3582</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4" t="s">
+        <v>3583</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>3584</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>3585</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>3586</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>3587</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>3588</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4" t="s">
+        <v>3589</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>3590</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>3590</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>3591</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>3592</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>3593</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="s">
+        <v>3594</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>3595</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>3596</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>3597</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>3598</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>3599</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="s">
+        <v>3600</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>3601</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>3602</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>3603</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>3604</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>3605</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4" t="s">
+        <v>3606</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>3607</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>3608</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>3609</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>3610</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>3611</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4" t="s">
+        <v>3612</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>3613</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>3614</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>3615</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>3616</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>3617</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4" t="s">
+        <v>3618</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>3619</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>3620</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>3621</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>3622</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>3623</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="K35"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>